<commit_message>
made output file work
</commit_message>
<xml_diff>
--- a/output.xlsx
+++ b/output.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E21"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,448 +436,263 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>id</t>
+          <t>firstname</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>type_id</t>
+          <t>lastname</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>name</t>
+          <t>teamname</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>id</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>name</t>
+          <t>yearjoined</t>
         </is>
       </c>
     </row>
     <row r="2">
-      <c r="A2" t="n">
-        <v>1</v>
-      </c>
-      <c r="B2" t="n">
-        <v>1</v>
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>Jrue</t>
+        </is>
+      </c>
+      <c r="B2" t="inlineStr">
+        <is>
+          <t>Holiday</t>
+        </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>Bagels</t>
+          <t>Philadelphia 76ers</t>
         </is>
       </c>
       <c r="D2" t="n">
-        <v>1</v>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>Bakery</t>
-        </is>
+        <v>2009</v>
       </c>
     </row>
     <row r="3">
-      <c r="A3" t="n">
-        <v>2</v>
-      </c>
-      <c r="B3" t="n">
-        <v>1</v>
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>Jrue</t>
+        </is>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>Holiday</t>
+        </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Bagels, raisin</t>
+          <t>New Orleans Pelicans</t>
         </is>
       </c>
       <c r="D3" t="n">
-        <v>1</v>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>Bakery</t>
-        </is>
+        <v>2013</v>
       </c>
     </row>
     <row r="4">
-      <c r="A4" t="n">
-        <v>3</v>
-      </c>
-      <c r="B4" t="n">
-        <v>1</v>
+      <c r="A4" t="inlineStr">
+        <is>
+          <t>Jrue</t>
+        </is>
+      </c>
+      <c r="B4" t="inlineStr">
+        <is>
+          <t>Holiday</t>
+        </is>
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>Bavarian Cream Pie</t>
+          <t>Milwaukee Bucks</t>
         </is>
       </c>
       <c r="D4" t="n">
-        <v>1</v>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>Bakery</t>
-        </is>
+        <v>2020</v>
       </c>
     </row>
     <row r="5">
-      <c r="A5" t="n">
-        <v>4</v>
-      </c>
-      <c r="B5" t="n">
-        <v>1</v>
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Jrue</t>
+        </is>
+      </c>
+      <c r="B5" t="inlineStr">
+        <is>
+          <t>Holiday</t>
+        </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>Bear Claws</t>
+          <t>Boston Celtics</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>1</v>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>Bakery</t>
-        </is>
+        <v>2023</v>
       </c>
     </row>
     <row r="6">
-      <c r="A6" t="n">
-        <v>5</v>
-      </c>
-      <c r="B6" t="n">
-        <v>1</v>
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Derrick</t>
+        </is>
+      </c>
+      <c r="B6" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>Black and White cookies</t>
+          <t>San Antonio Spurs</t>
         </is>
       </c>
       <c r="D6" t="n">
-        <v>1</v>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>Bakery</t>
-        </is>
+        <v>2017</v>
       </c>
     </row>
     <row r="7">
-      <c r="A7" t="n">
-        <v>6</v>
-      </c>
-      <c r="B7" t="n">
-        <v>1</v>
+      <c r="A7" t="inlineStr">
+        <is>
+          <t>Derrick</t>
+        </is>
+      </c>
+      <c r="B7" t="inlineStr">
+        <is>
+          <t>White</t>
+        </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>Bread (with nuts)</t>
+          <t>Boston Celtics</t>
         </is>
       </c>
       <c r="D7" t="n">
-        <v>1</v>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>Bakery</t>
-        </is>
+        <v>2022</v>
       </c>
     </row>
     <row r="8">
-      <c r="A8" t="n">
-        <v>7</v>
-      </c>
-      <c r="B8" t="n">
-        <v>1</v>
+      <c r="A8" t="inlineStr">
+        <is>
+          <t>Jaylen</t>
+        </is>
+      </c>
+      <c r="B8" t="inlineStr">
+        <is>
+          <t>Brown</t>
+        </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>Butterfingers</t>
+          <t>Boston Celtics</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>1</v>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>Bakery</t>
-        </is>
+        <v>2016</v>
       </c>
     </row>
     <row r="9">
-      <c r="A9" t="n">
-        <v>8</v>
-      </c>
-      <c r="B9" t="n">
-        <v>1</v>
+      <c r="A9" t="inlineStr">
+        <is>
+          <t>Jayson</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>Tatum</t>
+        </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>Carrot Cake</t>
+          <t>Boston Celtics</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>1</v>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>Bakery</t>
-        </is>
+        <v>2017</v>
       </c>
     </row>
     <row r="10">
-      <c r="A10" t="n">
-        <v>9</v>
-      </c>
-      <c r="B10" t="n">
-        <v>1</v>
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>Kristaps</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>Porzingis</t>
+        </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>Chips Ahoy Cookies</t>
+          <t>New York Knicks</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>1</v>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>Bakery</t>
-        </is>
+        <v>2015</v>
       </c>
     </row>
     <row r="11">
-      <c r="A11" t="n">
-        <v>10</v>
-      </c>
-      <c r="B11" t="n">
-        <v>1</v>
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>Kristaps</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>Porzingis</t>
+        </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>Chocolate Bobka</t>
+          <t>Dallas Mavericks</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>1</v>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>Bakery</t>
-        </is>
+        <v>2019</v>
       </c>
     </row>
     <row r="12">
-      <c r="A12" t="n">
-        <v>11</v>
-      </c>
-      <c r="B12" t="n">
-        <v>1</v>
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>Kristaps</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>Porzingis</t>
+        </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>Chocolate Eclairs</t>
+          <t>Washington Wizards</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>1</v>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>Bakery</t>
-        </is>
+        <v>2021</v>
       </c>
     </row>
     <row r="13">
-      <c r="A13" t="n">
-        <v>12</v>
-      </c>
-      <c r="B13" t="n">
-        <v>1</v>
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>Kristaps</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>Porzingis</t>
+        </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>Chocolate Cream Pie</t>
+          <t>Boston Celtics</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>1</v>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>Bakery</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="n">
-        <v>13</v>
-      </c>
-      <c r="B14" t="n">
-        <v>1</v>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>Cinnamon Bobka</t>
-        </is>
-      </c>
-      <c r="D14" t="n">
-        <v>1</v>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>Bakery</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="n">
-        <v>14</v>
-      </c>
-      <c r="B15" t="n">
-        <v>1</v>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>Cinnamon Swirls</t>
-        </is>
-      </c>
-      <c r="D15" t="n">
-        <v>1</v>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>Bakery</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" t="n">
-        <v>15</v>
-      </c>
-      <c r="B16" t="n">
-        <v>1</v>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>Cookie</t>
-        </is>
-      </c>
-      <c r="D16" t="n">
-        <v>1</v>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>Bakery</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" t="n">
-        <v>16</v>
-      </c>
-      <c r="B17" t="n">
-        <v>1</v>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>Crackers</t>
-        </is>
-      </c>
-      <c r="D17" t="n">
-        <v>1</v>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>Bakery</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" t="n">
-        <v>17</v>
-      </c>
-      <c r="B18" t="n">
-        <v>1</v>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>Cupcake</t>
-        </is>
-      </c>
-      <c r="D18" t="n">
-        <v>1</v>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>Bakery</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" t="n">
-        <v>18</v>
-      </c>
-      <c r="B19" t="n">
-        <v>1</v>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>Cupcakes</t>
-        </is>
-      </c>
-      <c r="D19" t="n">
-        <v>1</v>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>Bakery</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" t="n">
-        <v>19</v>
-      </c>
-      <c r="B20" t="n">
-        <v>1</v>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>Devils Food Cake</t>
-        </is>
-      </c>
-      <c r="D20" t="n">
-        <v>1</v>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>Bakery</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" t="n">
-        <v>20</v>
-      </c>
-      <c r="B21" t="n">
-        <v>1</v>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>Dinky Donuts</t>
-        </is>
-      </c>
-      <c r="D21" t="n">
-        <v>1</v>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>Bakery</t>
-        </is>
+        <v>2023</v>
       </c>
     </row>
   </sheetData>

</xml_diff>